<commit_message>
trying to do smthng
</commit_message>
<xml_diff>
--- a/labs/lab3/fluff_tablel3-l.xlsx
+++ b/labs/lab3/fluff_tablel3-l.xlsx
@@ -389,13 +389,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.4019546195653758</v>
+        <v>-0.05479815075587835</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01203952261077268</v>
+        <v>-0.043967052216493</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02995244245181393</v>
+        <v>0.8023455465196794</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -403,13 +403,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.01203952261077268</v>
+        <v>-0.043967052216493</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002845501024570513</v>
+        <v>0.0005085818044777701</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2363466656081883</v>
+        <v>0.01156733915145191</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -417,13 +417,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.002845501024570513</v>
+        <v>0.0005085818044777701</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0004768444727729637</v>
+        <v>-3.758094060735129e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1675783873052502</v>
+        <v>0.07389360035391107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -431,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0004768444727729637</v>
+        <v>-3.758094060735129e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>7.708574459985851e-05</v>
+        <v>-2.61509441301655e-06</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1616580436627201</v>
+        <v>0.06958565620640708</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -445,13 +445,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7.708574459985851e-05</v>
+        <v>-2.61509441301655e-06</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0001141398918208525</v>
+        <v>2.662474662962211e-07</v>
       </c>
       <c r="D6" t="n">
-        <v>1.480687413909497</v>
+        <v>0.101811798828747</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -459,13 +459,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0001141398918208525</v>
+        <v>2.662474662962211e-07</v>
       </c>
       <c r="C7" t="n">
-        <v>-6.06561447107079e-05</v>
+        <v>5.168764061203035e-08</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5314193288873127</v>
+        <v>0.1941338309470476</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -473,13 +473,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>-6.06561447107079e-05</v>
+        <v>5.168764061203035e-08</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0001257497812049979</v>
+        <v>-3.258101455294593e-09</v>
       </c>
       <c r="D8" t="n">
-        <v>2.073158157425702</v>
+        <v>0.06303443950460116</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -487,13 +487,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0001257497812049979</v>
+        <v>-3.258101455294593e-09</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.630235446273276e-05</v>
+        <v>-1.521550663241555e-09</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1296412153286898</v>
+        <v>0.4670053048130077</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -501,13 +501,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.630235446273276e-05</v>
+        <v>-1.521550663241555e-09</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001739980350020376</v>
+        <v>1.757871626040242e-11</v>
       </c>
       <c r="D10" t="n">
-        <v>10.67318437958135</v>
+        <v>0.01155315868546382</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -515,13 +515,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0001739980350020376</v>
+        <v>1.757871626040242e-11</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0003017891512065718</v>
+        <v>5.363054444984527e-11</v>
       </c>
       <c r="D11" t="n">
-        <v>1.734439996423165</v>
+        <v>3.05087946442669</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -529,13 +529,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0003017891512065718</v>
+        <v>5.363054444984527e-11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0002487650438505462</v>
+        <v>2.524758180300068e-12</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8243008168317784</v>
+        <v>0.04707687020893842</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -543,13 +543,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0002487650438505462</v>
+        <v>2.524758180300068e-12</v>
       </c>
       <c r="C13" t="n">
-        <v>-3.692852954731429e-05</v>
+        <v>-2.049249658853114e-12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1484474224179999</v>
+        <v>0.8116617562991952</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -557,13 +557,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.692852954731429e-05</v>
+        <v>-2.049249658853114e-12</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0005261256488121313</v>
+        <v>-2.410294186461215e-13</v>
       </c>
       <c r="D14" t="n">
-        <v>14.24713237330607</v>
+        <v>0.117618376855564</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -571,13 +571,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0005261256488121313</v>
+        <v>-2.410294186461215e-13</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.001114705549139811</v>
+        <v>7.949196856316121e-14</v>
       </c>
       <c r="D15" t="n">
-        <v>2.118705962456982</v>
+        <v>0.3298019345923537</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -585,13 +585,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.001114705549139811</v>
+        <v>7.949196856316121e-14</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.001644479261743159</v>
+        <v>1.720845688168993e-14</v>
       </c>
       <c r="D16" t="n">
-        <v>1.475258881605247</v>
+        <v>0.2164804469273743</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -599,13 +599,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.001644479261743159</v>
+        <v>1.720845688168993e-14</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.001933005607183763</v>
+        <v>-2.220446049250313e-15</v>
       </c>
       <c r="D17" t="n">
-        <v>1.175451495286577</v>
+        <v>0.1290322580645161</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -613,13 +613,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.001933005607183763</v>
+        <v>-2.220446049250313e-15</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.00180635148293129</v>
+        <v>-1.998401444325282e-15</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9344781392346821</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -627,13 +627,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.00180635148293129</v>
+        <v>-1.998401444325282e-15</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.001129084734272839</v>
+        <v>1.332267629550188e-15</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6250636960424759</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>